<commit_message>
📊 UPDATE: Refresh export reports with latest data
- Update CSV and Excel reports with current season data
- Ensure exports are properly organized in exports/ directory
- Reports include all processed weeks and current standings
</commit_message>
<xml_diff>
--- a/exports/skins_game_season_report.xlsx
+++ b/exports/skins_game_season_report.xlsx
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="H4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -1685,7 +1685,7 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1798,7 +1798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2635,6 +2635,466 @@
         </is>
       </c>
       <c r="E36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1005271556681232384</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>997251019148951552</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1125900327032598528</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1005301584701521920</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>865061949451403264</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1005271556681232384</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>997251019148951552</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1125900327032598528</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1005301584701521920</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>865061949451403264</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1005271556681232384</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>997251019148951552</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1125900327032598528</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1005301584701521920</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>865061949451403264</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1005271556681232384</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>997251019148951552</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1125900327032598528</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1005301584701521920</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>865061949451403264</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2676,7 +3136,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -2707,7 +3167,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-09 13:03:41</t>
+          <t>2025-09-09 13:20:27</t>
         </is>
       </c>
     </row>

</xml_diff>